<commit_message>
Dicionário, conceitual, e lógico-> Final
</commit_message>
<xml_diff>
--- a/Dicionário de dados(Merc. ViAna).xlsx
+++ b/Dicionário de dados(Merc. ViAna).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Documents\Projetos\Projetos Pessoais\Modelo Mercadinho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98188626-E522-435B-9AA0-A1ECF2C003EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E61C43-8FCF-4FE3-89F6-5E9CB4A5836D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4C9996F6-BD37-4BE8-8E4B-F3422DDB5909}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{4C9996F6-BD37-4BE8-8E4B-F3422DDB5909}"/>
   </bookViews>
   <sheets>
     <sheet name="DICIONÁRIO" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="174">
   <si>
     <t>DICIONÁRIO DE DADOS : MERCADINHO VIANA</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Registros, dados e valores e formas de pagamentos</t>
   </si>
   <si>
-    <t>Individuos para uma cardeneta</t>
-  </si>
-  <si>
     <t>Atributo</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>valor_venda</t>
   </si>
   <si>
-    <t>06 bytes</t>
-  </si>
-  <si>
     <t>valor de venda, que será repassado para os clientes finais</t>
   </si>
   <si>
@@ -382,20 +376,9 @@
     <t>bairro de endereço</t>
   </si>
   <si>
-    <t>Associativa</t>
-  </si>
-  <si>
     <t>Associação entre as entidade Produto e Fornecedor</t>
   </si>
   <si>
-    <t>Efetua
-É(ser)
-Composta</t>
-  </si>
-  <si>
-    <t>Compra</t>
-  </si>
-  <si>
     <t>produto_código_barras</t>
   </si>
   <si>
@@ -406,9 +389,6 @@
   </si>
   <si>
     <t>a data de fabricação do produto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 bytes</t>
   </si>
   <si>
     <t>produto_codigo_barras</t>
@@ -430,11 +410,6 @@
 Fornecedor</t>
   </si>
   <si>
-    <t>Categoria
-Prod_Forn
-Compra(Prod_Vend)</t>
-  </si>
-  <si>
     <t>Produto
 Categoria_Fornecedor</t>
   </si>
@@ -443,24 +418,10 @@
 Fornece</t>
   </si>
   <si>
-    <t>Operadora
-Compra(Prod_Vend)</t>
-  </si>
-  <si>
     <t>Cardeneta</t>
   </si>
   <si>
     <t>Compra(prod_vend)</t>
-  </si>
-  <si>
-    <t>Cardeneta
-Venda
-Produto</t>
-  </si>
-  <si>
-    <t>Contém
-Forma
-Composto</t>
   </si>
   <si>
     <t>Efetua</t>
@@ -474,11 +435,6 @@
 Fornece</t>
   </si>
   <si>
-    <t>Pertence
-Associativa
-Associativa</t>
-  </si>
-  <si>
     <t>Categoria_Fornecedor</t>
   </si>
   <si>
@@ -529,9 +485,6 @@
     <t>venda_id_venda</t>
   </si>
   <si>
-    <t>VARCHAR()</t>
-  </si>
-  <si>
     <t>contato_vendedor</t>
   </si>
   <si>
@@ -563,6 +516,70 @@
   </si>
   <si>
     <t>referencia a tabela operadora</t>
+  </si>
+  <si>
+    <t>Categoria
+Produto_Fornecedor
+Compra(Prod_Vend)</t>
+  </si>
+  <si>
+    <t>Pertence
+Fornece
+composta</t>
+  </si>
+  <si>
+    <t>Operadora
+Compra(Prod_Vend) Cardeneta</t>
+  </si>
+  <si>
+    <t>Efetua
+Formada
+Composta</t>
+  </si>
+  <si>
+    <t>Venda
+Produto</t>
+  </si>
+  <si>
+    <t>Forma
+Composto</t>
+  </si>
+  <si>
+    <t>Fornece
+Fornecido</t>
+  </si>
+  <si>
+    <t>Composta</t>
+  </si>
+  <si>
+    <t>Individuos que tem uma forma de pagamento diferente de cartão, mais a prazo.</t>
+  </si>
+  <si>
+    <t>100 bytes</t>
+  </si>
+  <si>
+    <t>03 bytes</t>
+  </si>
+  <si>
+    <t>DECIMAL(6,2)</t>
+  </si>
+  <si>
+    <t>01 bytes</t>
+  </si>
+  <si>
+    <t>02 bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04 bytes</t>
+  </si>
+  <si>
+    <t>quantiade de cadad unidade</t>
+  </si>
+  <si>
+    <t>valor_parcial</t>
+  </si>
+  <si>
+    <t>soma da quantidade de cada produto da compra</t>
   </si>
 </sst>
 </file>
@@ -717,6 +734,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -728,12 +751,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D592C8F-E7F4-49F2-91C1-083B84B7EDA5}">
   <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1070,12 +1087,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1084,16 +1101,16 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1102,10 +1119,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>8</v>
@@ -1116,10 +1133,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>9</v>
@@ -1130,10 +1147,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>10</v>
@@ -1141,86 +1158,86 @@
     </row>
     <row r="7" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>113</v>
+        <v>121</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55093CCB-F860-4A7D-8535-8F2D35AA042B}">
   <dimension ref="B1:F5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1251,63 +1268,63 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1323,7 +1340,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1338,284 +1355,284 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>32</v>
-      </c>
       <c r="E4" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>40</v>
+        <v>166</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="D8" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>18</v>
+        <v>169</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>22</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>18</v>
-      </c>
       <c r="E17" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1631,7 +1648,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1645,63 +1662,63 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -1724,7 +1741,7 @@
   <dimension ref="B1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1740,148 +1757,148 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="97.2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="83.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1910,63 +1927,63 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1998,80 +2015,80 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2104,7 @@
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2101,84 +2118,105 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>156</v>
+        <v>16</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="56.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2201,233 +2239,233 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2457,63 +2495,63 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>